<commit_message>
employee  projectType 新增search方法 并更新文档
</commit_message>
<xml_diff>
--- a/doc/接口文档.xlsx
+++ b/doc/接口文档.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="131" uniqueCount="104">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="143" uniqueCount="113">
   <si>
     <t>URL</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -462,12 +462,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>pageNum
-pageSize
-searchString</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>List&lt;ShopVo&gt;</t>
   </si>
   <si>
@@ -489,6 +483,53 @@
   </si>
   <si>
     <t>搜索</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>search</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>/projectType/search</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>搜索</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>/employee/search</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>pageNum
+pageSize
+searchString</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>pageNum
+pageSize
+searchString</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>搜索</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>/stockType/search</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>/stock/search</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>pageNum
+pageSize
+typeId
+searchString</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -871,11 +912,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:I30"/>
+  <dimension ref="A1:I34"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="F3" sqref="F3"/>
+      <pane ySplit="1" topLeftCell="A23" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="F30" sqref="F30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14" x14ac:dyDescent="0.3"/>
@@ -932,13 +973,13 @@
         <v>12</v>
       </c>
       <c r="F2" s="2" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="G2" s="2" t="s">
         <v>8</v>
       </c>
       <c r="H2" s="2" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
     </row>
     <row r="3" spans="1:9" ht="56" customHeight="1" x14ac:dyDescent="0.3">
@@ -1019,25 +1060,25 @@
         <v>97</v>
       </c>
       <c r="F6" s="2" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
     </row>
     <row r="7" spans="1:9" ht="42" x14ac:dyDescent="0.3">
       <c r="A7" s="3"/>
       <c r="B7" s="2" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="C7" s="2" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="D7" s="2" t="s">
         <v>13</v>
       </c>
       <c r="E7" s="2" t="s">
+        <v>107</v>
+      </c>
+      <c r="F7" s="2" t="s">
         <v>98</v>
-      </c>
-      <c r="F7" s="2" t="s">
-        <v>99</v>
       </c>
     </row>
     <row r="8" spans="1:9" ht="28" x14ac:dyDescent="0.3">
@@ -1060,321 +1101,369 @@
         <v>26</v>
       </c>
     </row>
-    <row r="9" spans="1:9" ht="56" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:9" ht="42" x14ac:dyDescent="0.3">
       <c r="A9" s="3"/>
       <c r="B9" s="2" t="s">
-        <v>25</v>
+        <v>105</v>
       </c>
       <c r="C9" s="2" t="s">
-        <v>27</v>
-      </c>
-      <c r="D9" s="2" t="s">
-        <v>13</v>
+        <v>106</v>
       </c>
       <c r="E9" s="2" t="s">
-        <v>92</v>
-      </c>
-      <c r="F9" s="2" t="s">
-        <v>28</v>
-      </c>
-      <c r="G9" s="2" t="s">
-        <v>8</v>
+        <v>108</v>
       </c>
     </row>
     <row r="10" spans="1:9" ht="56" x14ac:dyDescent="0.3">
       <c r="A10" s="3"/>
       <c r="B10" s="2" t="s">
-        <v>88</v>
+        <v>25</v>
       </c>
       <c r="C10" s="2" t="s">
-        <v>90</v>
+        <v>27</v>
+      </c>
+      <c r="D10" s="2" t="s">
+        <v>13</v>
       </c>
       <c r="E10" s="2" t="s">
-        <v>93</v>
-      </c>
-    </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.3">
+        <v>92</v>
+      </c>
+      <c r="F10" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="G10" s="2" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="11" spans="1:9" ht="56" x14ac:dyDescent="0.3">
       <c r="A11" s="3"/>
       <c r="B11" s="2" t="s">
+        <v>88</v>
+      </c>
+      <c r="C11" s="2" t="s">
+        <v>90</v>
+      </c>
+      <c r="E11" s="2" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="12" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A12" s="3"/>
+      <c r="B12" s="2" t="s">
         <v>89</v>
       </c>
-      <c r="C11" s="2" t="s">
+      <c r="C12" s="2" t="s">
         <v>91</v>
       </c>
-      <c r="E11" s="2" t="s">
+      <c r="E12" s="2" t="s">
         <v>94</v>
       </c>
     </row>
-    <row r="12" spans="1:9" ht="42" x14ac:dyDescent="0.3">
-      <c r="A12" s="2" t="s">
+    <row r="13" spans="1:9" ht="42" x14ac:dyDescent="0.3">
+      <c r="A13" s="2" t="s">
         <v>30</v>
       </c>
-      <c r="B12" s="2" t="s">
+      <c r="B13" s="2" t="s">
         <v>31</v>
       </c>
-      <c r="C12" s="2" t="s">
+      <c r="C13" s="2" t="s">
         <v>32</v>
       </c>
-      <c r="D12" s="2" t="s">
+      <c r="D13" s="2" t="s">
         <v>33</v>
       </c>
-      <c r="E12" s="2" t="s">
+      <c r="E13" s="2" t="s">
         <v>34</v>
       </c>
-      <c r="G12" s="2" t="s">
+      <c r="G13" s="2" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="13" spans="1:9" ht="84" x14ac:dyDescent="0.3">
-      <c r="A13" s="3" t="s">
+    <row r="14" spans="1:9" ht="84" x14ac:dyDescent="0.3">
+      <c r="A14" s="3" t="s">
         <v>37</v>
       </c>
-      <c r="B13" s="2" t="s">
+      <c r="B14" s="2" t="s">
         <v>36</v>
       </c>
-      <c r="C13" s="2" t="s">
+      <c r="C14" s="2" t="s">
         <v>38</v>
       </c>
-      <c r="F13" s="2" t="s">
+      <c r="F14" s="2" t="s">
         <v>40</v>
       </c>
-      <c r="H13" s="2" t="s">
+      <c r="H14" s="2" t="s">
         <v>41</v>
       </c>
-      <c r="I13" s="2" t="s">
+      <c r="I14" s="2" t="s">
         <v>42</v>
       </c>
     </row>
-    <row r="14" spans="1:9" ht="28" x14ac:dyDescent="0.3">
-      <c r="A14" s="3"/>
-      <c r="B14" s="2" t="s">
-        <v>43</v>
-      </c>
-      <c r="C14" s="2" t="s">
-        <v>44</v>
-      </c>
-      <c r="E14" s="2" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="15" spans="1:9" ht="42" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:9" ht="28" x14ac:dyDescent="0.3">
       <c r="A15" s="3"/>
       <c r="B15" s="2" t="s">
-        <v>46</v>
+        <v>43</v>
       </c>
       <c r="C15" s="2" t="s">
-        <v>47</v>
+        <v>44</v>
       </c>
       <c r="E15" s="2" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="16" spans="1:9" x14ac:dyDescent="0.3">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="16" spans="1:9" ht="42" x14ac:dyDescent="0.3">
       <c r="A16" s="3"/>
       <c r="B16" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="C16" s="2" t="s">
+        <v>47</v>
+      </c>
+      <c r="E16" s="2" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="17" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A17" s="3"/>
+      <c r="B17" s="2" t="s">
         <v>49</v>
       </c>
-      <c r="C16" s="2" t="s">
+      <c r="C17" s="2" t="s">
         <v>50</v>
       </c>
-      <c r="E16" s="2" t="s">
+      <c r="E17" s="2" t="s">
         <v>51</v>
       </c>
     </row>
-    <row r="17" spans="1:8" ht="42" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A17" s="3" t="s">
-        <v>52</v>
-      </c>
-      <c r="B17" s="2" t="s">
-        <v>36</v>
-      </c>
-      <c r="C17" s="2" t="s">
-        <v>55</v>
-      </c>
-      <c r="F17" s="2" t="s">
-        <v>59</v>
-      </c>
-      <c r="H17" s="2" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="18" spans="1:8" ht="42" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:8" ht="42" x14ac:dyDescent="0.3">
       <c r="A18" s="3"/>
       <c r="B18" s="2" t="s">
-        <v>61</v>
+        <v>103</v>
       </c>
       <c r="C18" s="2" t="s">
-        <v>62</v>
+        <v>104</v>
       </c>
       <c r="E18" s="2" t="s">
-        <v>63</v>
-      </c>
-      <c r="F18" s="2" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="19" spans="1:8" ht="42" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A19" s="3" t="s">
+        <v>52</v>
+      </c>
+      <c r="B19" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="C19" s="2" t="s">
+        <v>55</v>
+      </c>
+      <c r="F19" s="2" t="s">
         <v>59</v>
       </c>
-    </row>
-    <row r="19" spans="1:8" ht="28" x14ac:dyDescent="0.3">
-      <c r="A19" s="3"/>
-      <c r="B19" s="2" t="s">
-        <v>43</v>
-      </c>
-      <c r="C19" s="2" t="s">
-        <v>56</v>
-      </c>
-      <c r="E19" s="2" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="20" spans="1:8" ht="28" x14ac:dyDescent="0.3">
+      <c r="H19" s="2" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="20" spans="1:8" ht="42" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A20" s="3"/>
       <c r="B20" s="2" t="s">
-        <v>53</v>
+        <v>61</v>
       </c>
       <c r="C20" s="2" t="s">
-        <v>57</v>
+        <v>62</v>
       </c>
       <c r="E20" s="2" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="21" spans="1:8" x14ac:dyDescent="0.3">
+        <v>63</v>
+      </c>
+      <c r="F20" s="2" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="21" spans="1:8" ht="28" x14ac:dyDescent="0.3">
       <c r="A21" s="3"/>
       <c r="B21" s="2" t="s">
-        <v>54</v>
+        <v>43</v>
       </c>
       <c r="C21" s="2" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="E21" s="2" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="22" spans="1:8" ht="42" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A22" s="3" t="s">
-        <v>65</v>
-      </c>
+        <v>64</v>
+      </c>
+    </row>
+    <row r="22" spans="1:8" ht="28" x14ac:dyDescent="0.3">
+      <c r="A22" s="3"/>
       <c r="B22" s="2" t="s">
-        <v>36</v>
+        <v>53</v>
       </c>
       <c r="C22" s="2" t="s">
-        <v>67</v>
-      </c>
-      <c r="F22" s="2" t="s">
-        <v>71</v>
-      </c>
-      <c r="H22" s="2" t="s">
-        <v>72</v>
+        <v>57</v>
+      </c>
+      <c r="E22" s="2" t="s">
+        <v>64</v>
       </c>
     </row>
     <row r="23" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A23" s="3"/>
       <c r="B23" s="2" t="s">
-        <v>43</v>
+        <v>54</v>
       </c>
       <c r="C23" s="2" t="s">
-        <v>68</v>
+        <v>58</v>
       </c>
       <c r="E23" s="2" t="s">
-        <v>73</v>
-      </c>
-    </row>
-    <row r="24" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A24" s="3"/>
+        <v>51</v>
+      </c>
+    </row>
+    <row r="24" spans="1:8" ht="42" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A24" s="3" t="s">
+        <v>65</v>
+      </c>
       <c r="B24" s="2" t="s">
-        <v>53</v>
+        <v>36</v>
       </c>
       <c r="C24" s="2" t="s">
-        <v>69</v>
-      </c>
-      <c r="E24" s="2" t="s">
-        <v>73</v>
-      </c>
-    </row>
-    <row r="25" spans="1:8" x14ac:dyDescent="0.3">
+        <v>67</v>
+      </c>
+      <c r="F24" s="2" t="s">
+        <v>71</v>
+      </c>
+      <c r="H24" s="2" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="25" spans="1:8" ht="42" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A25" s="3"/>
       <c r="B25" s="2" t="s">
-        <v>66</v>
+        <v>109</v>
       </c>
       <c r="C25" s="2" t="s">
-        <v>70</v>
+        <v>110</v>
       </c>
       <c r="E25" s="2" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="26" spans="1:8" ht="84" x14ac:dyDescent="0.3">
-      <c r="A26" s="3" t="s">
-        <v>74</v>
-      </c>
+        <v>108</v>
+      </c>
+    </row>
+    <row r="26" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A26" s="3"/>
       <c r="B26" s="2" t="s">
-        <v>36</v>
+        <v>43</v>
       </c>
       <c r="C26" s="2" t="s">
-        <v>76</v>
-      </c>
-      <c r="F26" s="2" t="s">
-        <v>82</v>
-      </c>
-      <c r="H26" s="2" t="s">
-        <v>83</v>
-      </c>
-    </row>
-    <row r="27" spans="1:8" ht="28" x14ac:dyDescent="0.3">
+        <v>68</v>
+      </c>
+      <c r="E26" s="2" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="27" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A27" s="3"/>
       <c r="B27" s="2" t="s">
-        <v>80</v>
+        <v>53</v>
       </c>
       <c r="C27" s="2" t="s">
-        <v>81</v>
-      </c>
-      <c r="F27" s="2" t="s">
-        <v>82</v>
-      </c>
-    </row>
-    <row r="28" spans="1:8" ht="56" x14ac:dyDescent="0.3">
+        <v>69</v>
+      </c>
+      <c r="E27" s="2" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="28" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A28" s="3"/>
       <c r="B28" s="2" t="s">
-        <v>43</v>
+        <v>66</v>
       </c>
       <c r="C28" s="2" t="s">
-        <v>77</v>
+        <v>70</v>
       </c>
       <c r="E28" s="2" t="s">
-        <v>84</v>
-      </c>
-    </row>
-    <row r="29" spans="1:8" ht="56" x14ac:dyDescent="0.3">
-      <c r="A29" s="3"/>
+        <v>51</v>
+      </c>
+    </row>
+    <row r="29" spans="1:8" ht="84" x14ac:dyDescent="0.3">
+      <c r="A29" s="3" t="s">
+        <v>74</v>
+      </c>
       <c r="B29" s="2" t="s">
-        <v>75</v>
+        <v>36</v>
       </c>
       <c r="C29" s="2" t="s">
-        <v>78</v>
-      </c>
-      <c r="E29" s="2" t="s">
-        <v>84</v>
-      </c>
-    </row>
-    <row r="30" spans="1:8" x14ac:dyDescent="0.3">
+        <v>76</v>
+      </c>
+      <c r="F29" s="2" t="s">
+        <v>82</v>
+      </c>
+      <c r="H29" s="2" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="30" spans="1:8" ht="56" x14ac:dyDescent="0.3">
       <c r="A30" s="3"/>
       <c r="B30" s="2" t="s">
+        <v>105</v>
+      </c>
+      <c r="C30" s="2" t="s">
+        <v>111</v>
+      </c>
+      <c r="E30" s="2" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="31" spans="1:8" ht="28" x14ac:dyDescent="0.3">
+      <c r="A31" s="3"/>
+      <c r="B31" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="C31" s="2" t="s">
+        <v>81</v>
+      </c>
+      <c r="F31" s="2" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="32" spans="1:8" ht="56" x14ac:dyDescent="0.3">
+      <c r="A32" s="3"/>
+      <c r="B32" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="C32" s="2" t="s">
+        <v>77</v>
+      </c>
+      <c r="E32" s="2" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="33" spans="1:5" ht="56" x14ac:dyDescent="0.3">
+      <c r="A33" s="3"/>
+      <c r="B33" s="2" t="s">
+        <v>75</v>
+      </c>
+      <c r="C33" s="2" t="s">
+        <v>78</v>
+      </c>
+      <c r="E33" s="2" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="34" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A34" s="3"/>
+      <c r="B34" s="2" t="s">
         <v>66</v>
       </c>
-      <c r="C30" s="2" t="s">
+      <c r="C34" s="2" t="s">
         <v>79</v>
       </c>
-      <c r="E30" s="2" t="s">
+      <c r="E34" s="2" t="s">
         <v>51</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="6">
-    <mergeCell ref="A22:A25"/>
-    <mergeCell ref="A26:A30"/>
-    <mergeCell ref="A13:A16"/>
-    <mergeCell ref="A17:A21"/>
-    <mergeCell ref="A8:A11"/>
     <mergeCell ref="A2:A7"/>
+    <mergeCell ref="A14:A18"/>
+    <mergeCell ref="A24:A28"/>
+    <mergeCell ref="A29:A34"/>
+    <mergeCell ref="A19:A23"/>
+    <mergeCell ref="A8:A12"/>
   </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>